<commit_message>
audio files have japanese title
</commit_message>
<xml_diff>
--- a/book.xlsx
+++ b/book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miroc\FlashCards\Flash_Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44CE915-2091-4725-945C-08B6F26CAA65}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CCC846-ED0D-4010-9FFB-CFC7972EC4D9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4035" yWindow="615" windowWidth="14385" windowHeight="11985" activeTab="3" xr2:uid="{77373029-EA19-3040-86B1-92EFA1594428}"/>
+    <workbookView xWindow="12765" yWindow="2475" windowWidth="14385" windowHeight="11985" activeTab="3" xr2:uid="{77373029-EA19-3040-86B1-92EFA1594428}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="478">
   <si>
     <t>underlay</t>
     <phoneticPr fontId="1"/>
@@ -2431,129 +2431,6 @@
     <rPh sb="3" eb="4">
       <t>チ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>temporary</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>臨時の、仮の</t>
-    <rPh sb="0" eb="2">
-      <t>リンジ</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>カリ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>stroke</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>打つこと、[心臓の]鼓動、脳卒中</t>
-    <rPh sb="0" eb="1">
-      <t>ウ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>シンゾウ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>コドウ</t>
-    </rPh>
-    <rPh sb="13" eb="16">
-      <t>ノウソッチュウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>戦術</t>
-    <rPh sb="0" eb="2">
-      <t>センジュツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>disturb</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>邪魔をする、妨げる</t>
-    <rPh sb="0" eb="2">
-      <t>ジャマ</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>サマタ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>incidental</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>付随的な、偶発的な</t>
-    <rPh sb="0" eb="3">
-      <t>フズイテキ</t>
-    </rPh>
-    <rPh sb="5" eb="8">
-      <t>グウハツテキ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>eternal</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>永遠の</t>
-    <rPh sb="0" eb="2">
-      <t>エイエン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>nearly</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ほとんど</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>profession</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[専門的]職業</t>
-    <rPh sb="1" eb="4">
-      <t>センモンテキ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>ショクギョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>disorder</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>混乱、無秩序、病気</t>
-    <rPh sb="0" eb="2">
-      <t>コンラン</t>
-    </rPh>
-    <rPh sb="3" eb="6">
-      <t>ムチツジョ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>ビョウキ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>tactic</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -4579,7 +4456,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="A1:B9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -4884,10 +4761,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091618A3-A297-4EFA-8E3F-3A2797E2E2AB}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -4924,78 +4801,6 @@
         <v>477</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>478</v>
-      </c>
-      <c r="B5" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>480</v>
-      </c>
-      <c r="B6" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>495</v>
-      </c>
-      <c r="B7" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>493</v>
-      </c>
-      <c r="B8" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>483</v>
-      </c>
-      <c r="B9" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>485</v>
-      </c>
-      <c r="B10" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>487</v>
-      </c>
-      <c r="B11" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>489</v>
-      </c>
-      <c r="B12" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>491</v>
-      </c>
-      <c r="B13" t="s">
-        <v>492</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>